<commit_message>
Chore : entry_path 수정
</commit_message>
<xml_diff>
--- a/STEM 관심사, 직무, 롤모델 연결.xlsx
+++ b/STEM 관심사, 직무, 롤모델 연결.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\owner\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\taeky\github\HERETHON5\2025-herethon-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0106EB2C-CD67-4340-98EF-BB858F130C5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A18548-7EFA-4661-AC69-71B4D7D3DAF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="384" yWindow="384" windowWidth="14532" windowHeight="8880" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="01_관심사 태그 마스터" sheetId="1" r:id="rId1"/>
@@ -180,9 +180,6 @@
     <t>환경공학, 통계학</t>
   </si>
   <si>
-    <t>공대 졸업 후 환경 연구소 또는 ESG 관련 인턴십</t>
-  </si>
-  <si>
     <t>#환경 #데이터 #기후</t>
   </si>
   <si>
@@ -216,9 +213,6 @@
     <t>산업공학, 컴퓨터공학</t>
   </si>
   <si>
-    <t>컴공/산업공학 기반 AI 스타트업 인턴 or 기획 포지션 경험</t>
-  </si>
-  <si>
     <t>#AI #기획 #트렌드</t>
   </si>
   <si>
@@ -252,9 +246,6 @@
     <t>심리학, 인지과학, 디자인학</t>
   </si>
   <si>
-    <t>UX 리서치 인턴십 또는 디자인 관련 프로젝트 참여</t>
-  </si>
-  <si>
     <t>#UX #사용자 #분석</t>
   </si>
   <si>
@@ -312,9 +303,6 @@
     <t>컴퓨터공학, 정보시스템</t>
   </si>
   <si>
-    <t>개발 공부 후 커뮤니티 플랫폼 스타트업 또는 오픈소스 커뮤니티 참여</t>
-  </si>
-  <si>
     <t>#커뮤니티 #개발 #네트워킹</t>
   </si>
   <si>
@@ -342,9 +330,6 @@
     <t>경영학, 통계학, 환경공학</t>
   </si>
   <si>
-    <t>ESG 컨설팅 인턴 또는 지속가능성 관련 공공기관/기업 데이터팀</t>
-  </si>
-  <si>
     <t>#ESG #환경 #데이터</t>
   </si>
   <si>
@@ -369,9 +354,6 @@
     <t>보건학, UX디자인, 디지털헬스케어학</t>
   </si>
   <si>
-    <t>디지털 헬스케어 스타트업 인턴, 관련 해커톤 또는 공모전 참가</t>
-  </si>
-  <si>
     <t>#건강 #앱기획 #웰니스</t>
   </si>
   <si>
@@ -396,9 +378,6 @@
     <t>패션학, 데이터사이언스, 컴퓨터공학</t>
   </si>
   <si>
-    <t>AI 프로젝트 경험 후 패션 리서치 스타트업 or 브랜드 분석팀 참여</t>
-  </si>
-  <si>
     <t>#패션 #AI #트렌드</t>
   </si>
   <si>
@@ -426,9 +405,6 @@
     <t>환경과학, 수학, 기후과학</t>
   </si>
   <si>
-    <t>시뮬레이션 소프트웨어 툴 학습 후 공공기관 또는 연구소 인턴십 경험</t>
-  </si>
-  <si>
     <t>#시뮬레이션 #기후 #수학</t>
   </si>
   <si>
@@ -607,6 +583,353 @@
   </si>
   <si>
     <t>Soft_Skills</t>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <t>공대 졸업 후 환경 연구소, ESG 관련 인턴십</t>
+  </si>
+  <si>
+    <t>컴공/산업공학 기반 AI 스타트업 인턴, 기획 포지션 경험</t>
+  </si>
+  <si>
+    <t>UX 리서치 인턴십, 디자인 관련 프로젝트 참여</t>
+  </si>
+  <si>
+    <t>개발 공부 후 커뮤니티 플랫폼 스타트업, 오픈소스 커뮤니티 참여</t>
+  </si>
+  <si>
+    <t>ESG 컨설팅 인턴, 지속가능성 관련 공공기관/기업 데이터팀</t>
+  </si>
+  <si>
+    <t>디지털 헬스케어 스타트업 인턴, 관련 해커톤, 공모전 참가</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>시뮬레이션</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>소프트웨어</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>툴</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>학습</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>공공기관</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>연구소</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>인턴십</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경험</t>
+    </r>
+    <phoneticPr fontId="8" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">AI </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>프로젝트</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>경험 후</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>패션</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>리서치</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>스타트업</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>브랜드</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>분석팀</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="맑은 고딕"/>
+        <family val="3"/>
+        <charset val="129"/>
+      </rPr>
+      <t>참여</t>
+    </r>
     <phoneticPr fontId="8" type="noConversion"/>
   </si>
 </sst>
@@ -617,7 +940,7 @@
   <numFmts count="1">
     <numFmt numFmtId="176" formatCode="m\,\ d"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -684,6 +1007,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -693,7 +1038,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -701,11 +1046,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -725,6 +1085,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -948,13 +1314,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="16.44140625" customWidth="1"/>
     <col min="3" max="3" width="38.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -965,7 +1331,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -976,7 +1342,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -987,7 +1353,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -998,7 +1364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -1009,7 +1375,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -1020,7 +1386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -1031,7 +1397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -1042,7 +1408,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -1053,7 +1419,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1064,7 +1430,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1075,7 +1441,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -1087,7 +1453,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -1098,7 +1464,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -1109,7 +1475,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="2">
         <v>14</v>
       </c>
@@ -1120,7 +1486,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16" s="2">
         <v>15</v>
       </c>
@@ -1131,7 +1497,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="7:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="7:9">
       <c r="G31" s="3"/>
       <c r="H31" s="3"/>
       <c r="I31" s="3"/>
@@ -1150,10 +1516,10 @@
   <dimension ref="A1:N30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="2" max="2" width="15.44140625" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
@@ -1166,7 +1532,7 @@
     <col min="12" max="12" width="17.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="13.8" thickBot="1">
       <c r="A1" s="3" t="s">
         <v>33</v>
       </c>
@@ -1186,7 +1552,7 @@
         <v>38</v>
       </c>
       <c r="G1" s="11" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>39</v>
@@ -1208,7 +1574,7 @@
       </c>
       <c r="N1" s="3"/>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="13.8" thickBot="1">
       <c r="A2" s="2" t="s">
         <v>45</v>
       </c>
@@ -1233,105 +1599,105 @@
       <c r="H2" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="K2" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="2" t="s">
+    </row>
+    <row r="3" spans="1:14" ht="13.8" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C3" s="2">
         <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="G3" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="G3" s="5" t="s">
+      <c r="H3" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="I3" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="J3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="K3" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="J3" s="2" t="s">
+      <c r="L3" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="K3" s="2" t="s">
+      <c r="M3" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="L3" s="2" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="13.8" thickBot="1">
+      <c r="A4" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>70</v>
       </c>
       <c r="C4" s="2">
         <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="G4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="H4" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="I4" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="J4" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="K4" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="L4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="2" t="s">
+      <c r="M4" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="K4" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M4" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:14" ht="13.8" thickBot="1">
       <c r="A5" s="2" t="s">
         <v>45</v>
       </c>
@@ -1342,78 +1708,78 @@
         <v>104</v>
       </c>
       <c r="D5" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="2" t="s">
+      <c r="H5" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="I5" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="G5" s="5" t="s">
+      <c r="J5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="K5" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I5" s="2" t="s">
+      <c r="L5" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="J5" s="2" t="s">
+      <c r="M5" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="K5" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="M5" s="6" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:14" ht="27" thickBot="1">
       <c r="A6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C6" s="2">
         <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="J6" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="K6" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="L6" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="I6" s="2" t="s">
+      <c r="M6" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="J6" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="M6" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:14" ht="27" thickBot="1">
       <c r="A7" s="2" t="s">
         <v>45</v>
       </c>
@@ -1424,119 +1790,119 @@
         <v>106</v>
       </c>
       <c r="D7" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="I7" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="J7" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="K7" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="L7" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="H7" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="M7" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="13.8" thickBot="1">
       <c r="A8" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C8" s="2">
         <v>107</v>
       </c>
       <c r="D8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="J8" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="K8" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="L8" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="M8" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="G8" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>116</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="M8" s="2" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:14" ht="31.8" thickBot="1">
       <c r="A9" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C9" s="2">
         <v>108</v>
       </c>
       <c r="D9" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="I9" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="K9" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="L9" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="M9" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>127</v>
-      </c>
-      <c r="M9" s="6" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:14" ht="31.8" thickBot="1">
       <c r="A10" s="2" t="s">
         <v>45</v>
       </c>
@@ -1547,85 +1913,85 @@
         <v>109</v>
       </c>
       <c r="D10" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>193</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="M10" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>131</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>132</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>136</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="M10" s="2" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:14" ht="27" thickBot="1">
       <c r="A11" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="C11" s="2">
         <v>110</v>
       </c>
       <c r="D11" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>135</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="M11" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="E11" s="2" t="s">
-        <v>139</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>141</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>142</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>143</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>144</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="L11" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="M11" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:14" ht="13.2">
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" ht="15.75" customHeight="1">
       <c r="G15" s="7"/>
     </row>
-    <row r="16" spans="1:14" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" ht="17.399999999999999">
       <c r="A16" s="3"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
@@ -1638,16 +2004,16 @@
       <c r="L16" s="3"/>
       <c r="M16" s="3"/>
     </row>
-    <row r="17" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" ht="17.399999999999999">
       <c r="G17" s="8"/>
     </row>
-    <row r="18" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" ht="17.399999999999999">
       <c r="G18" s="8"/>
     </row>
-    <row r="19" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" ht="17.399999999999999">
       <c r="G19" s="8"/>
     </row>
-    <row r="20" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" ht="17.399999999999999">
       <c r="A20" s="3"/>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
@@ -1659,46 +2025,47 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" ht="17.399999999999999">
       <c r="G21" s="8"/>
       <c r="L21" s="9"/>
     </row>
-    <row r="22" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" ht="17.399999999999999">
       <c r="G22" s="8"/>
       <c r="L22" s="9"/>
     </row>
-    <row r="23" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" ht="17.399999999999999">
       <c r="G23" s="8"/>
       <c r="L23" s="9"/>
     </row>
-    <row r="24" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" ht="17.399999999999999">
       <c r="G24" s="8"/>
       <c r="L24" s="9"/>
     </row>
-    <row r="25" spans="1:12" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" ht="17.399999999999999">
       <c r="E25" s="8"/>
       <c r="F25" s="8"/>
       <c r="G25" s="8"/>
       <c r="L25" s="9"/>
     </row>
-    <row r="26" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="13.2">
       <c r="L26" s="9"/>
     </row>
-    <row r="27" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" ht="13.2">
       <c r="L27" s="9"/>
     </row>
-    <row r="28" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" ht="13.2">
       <c r="L28" s="9"/>
     </row>
-    <row r="29" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" ht="13.2">
       <c r="L29" s="9"/>
     </row>
-    <row r="30" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" ht="13.2">
       <c r="L30" s="9"/>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1711,19 +2078,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="5" max="5" width="45.109375" customWidth="1"/>
     <col min="6" max="6" width="66" customWidth="1"/>
     <col min="7" max="7" width="38.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="3" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>35</v>
@@ -1732,267 +2099,267 @@
         <v>44</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C2" s="2">
         <v>101</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C3" s="2">
         <v>102</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C4" s="2">
         <v>103</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="2">
         <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C5" s="2">
         <v>104</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="2">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C6" s="2">
         <v>105</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C7" s="2">
         <v>101</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
       <c r="A8" s="2">
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C8" s="2">
         <v>106</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="2">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C9" s="2">
         <v>107</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
       <c r="A10" s="2">
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C10" s="2">
         <v>108</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
       <c r="A11" s="2">
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C11" s="2">
         <v>109</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="21" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="5:7">
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>

</xml_diff>